<commit_message>
Adiciona melhorias em bolao-template.html e atualiza lotofacil/config.json
- Ajustes e melhorias na interface do template de bolão
- Atualização dos dados de configuração da lotofacil
</commit_message>
<xml_diff>
--- a/lotofacil/Bolão independencia - 130.xlsx
+++ b/lotofacil/Bolão independencia - 130.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Desktop\Bolão\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Desktop\Bolão\Bolao_Mega\lotofacil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A996DE80-711B-4F94-80BD-0BCE6941B721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C815C12-E6E1-4DCB-81D2-EB4B610C0A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14610" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="13 cotas(10 Jogos)" sheetId="1" r:id="rId1"/>
+    <sheet name="13 cotas" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>

</xml_diff>